<commit_message>
first of DEC update
</commit_message>
<xml_diff>
--- a/Word skill.xlsx
+++ b/Word skill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xre22\OneDrive\Desktop\Data sciense\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26AF453-90FE-48EA-8C0F-DAFFC8AF6763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C35FD8-21F8-4C28-8C0D-C54B308A41AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="4770" windowWidth="13140" windowHeight="8925" xr2:uid="{FBACF5EB-20B7-4407-9D0F-78415D039E96}"/>
+    <workbookView xWindow="15660" yWindow="390" windowWidth="13140" windowHeight="8925" xr2:uid="{FBACF5EB-20B7-4407-9D0F-78415D039E96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="535">
   <si>
     <t>Asymmetrical</t>
   </si>
@@ -1072,9 +1072,6 @@
   </si>
   <si>
     <t xml:space="preserve">nifty </t>
-  </si>
-  <si>
-    <t>زیبا</t>
   </si>
   <si>
     <t>inference</t>
@@ -1629,6 +1626,24 @@
   </si>
   <si>
     <t>سبیل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intrinsic </t>
+  </si>
+  <si>
+    <t>زیبا، جالب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderately </t>
+  </si>
+  <si>
+    <t>نسبتا</t>
+  </si>
+  <si>
+    <t xml:space="preserve">surpass </t>
+  </si>
+  <si>
+    <t>پیشی گرفتن</t>
   </si>
 </sst>
 </file>
@@ -2321,8 +2336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8103EE8-8652-4065-9906-2F66BB4C7AFE}">
   <dimension ref="A1:B394"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A273" workbookViewId="0">
-      <selection activeCell="B283" sqref="B283"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A280" workbookViewId="0">
+      <selection activeCell="B286" sqref="B286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3776,95 +3791,95 @@
         <v>345</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>346</v>
+        <v>530</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="44.1" customHeight="1">
       <c r="A182" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B182" s="15" t="s">
         <v>347</v>
-      </c>
-      <c r="B182" s="15" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="44.1" customHeight="1">
       <c r="A183" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B183" s="7" t="s">
         <v>349</v>
-      </c>
-      <c r="B183" s="7" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="44.1" customHeight="1">
       <c r="A184" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B184" s="7" t="s">
         <v>351</v>
-      </c>
-      <c r="B184" s="7" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="44.1" customHeight="1">
       <c r="A185" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B185" s="7" t="s">
         <v>353</v>
-      </c>
-      <c r="B185" s="7" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="44.1" customHeight="1">
       <c r="A186" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="B186" s="7" t="s">
         <v>355</v>
-      </c>
-      <c r="B186" s="7" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="44.1" customHeight="1">
       <c r="A187" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B187" s="7" t="s">
         <v>357</v>
-      </c>
-      <c r="B187" s="7" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="44.1" customHeight="1">
       <c r="A188" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B188" s="7" t="s">
         <v>359</v>
-      </c>
-      <c r="B188" s="7" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="44.1" customHeight="1">
       <c r="A189" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B189" s="7" t="s">
         <v>361</v>
-      </c>
-      <c r="B189" s="7" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="44.1" customHeight="1">
       <c r="A190" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B190" s="7" t="s">
         <v>363</v>
-      </c>
-      <c r="B190" s="7" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="44.1" customHeight="1">
       <c r="A191" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B191" s="7" t="s">
         <v>365</v>
-      </c>
-      <c r="B191" s="7" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="44.1" customHeight="1">
       <c r="A192" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B192" s="7" t="s">
         <v>367</v>
-      </c>
-      <c r="B192" s="7" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="44.1" customHeight="1">
@@ -3877,127 +3892,127 @@
     </row>
     <row r="194" spans="1:2" ht="44.1" customHeight="1">
       <c r="A194" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B194" s="7" t="s">
         <v>369</v>
-      </c>
-      <c r="B194" s="7" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="44.1" customHeight="1">
       <c r="A195" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B195" s="7" t="s">
         <v>371</v>
-      </c>
-      <c r="B195" s="7" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="44.1" customHeight="1">
       <c r="A196" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="B196" s="7" t="s">
         <v>373</v>
-      </c>
-      <c r="B196" s="7" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="44.1" customHeight="1">
       <c r="A197" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B197" s="7" t="s">
         <v>375</v>
-      </c>
-      <c r="B197" s="7" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="44.1" customHeight="1">
       <c r="A198" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B198" s="7" t="s">
         <v>377</v>
-      </c>
-      <c r="B198" s="7" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="44.1" customHeight="1">
       <c r="A199" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B199" s="7" t="s">
         <v>379</v>
-      </c>
-      <c r="B199" s="7" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="44.1" customHeight="1">
       <c r="A200" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B200" s="7" t="s">
         <v>381</v>
-      </c>
-      <c r="B200" s="7" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="44.1" customHeight="1">
       <c r="A201" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B201" s="7" t="s">
         <v>383</v>
-      </c>
-      <c r="B201" s="7" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="44.1" customHeight="1">
       <c r="A202" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B202" s="7" t="s">
         <v>377</v>
-      </c>
-      <c r="B202" s="7" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="44.1" customHeight="1">
       <c r="A203" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B203" s="7" t="s">
         <v>385</v>
-      </c>
-      <c r="B203" s="7" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="89.25" customHeight="1">
       <c r="A204" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="B204" s="16" t="s">
         <v>387</v>
-      </c>
-      <c r="B204" s="16" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="44.1" customHeight="1">
       <c r="A205" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B205" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="B205" s="7" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="44.1" customHeight="1">
       <c r="A206" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B206" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="44.1" customHeight="1">
       <c r="A207" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B207" s="7" t="s">
         <v>392</v>
-      </c>
-      <c r="B207" s="7" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="44.1" customHeight="1">
       <c r="A208" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B208" s="7" t="s">
         <v>394</v>
-      </c>
-      <c r="B208" s="7" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="44.1" customHeight="1">
       <c r="A209" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B209" s="7" t="s">
         <v>268</v>
@@ -4005,18 +4020,18 @@
     </row>
     <row r="210" spans="1:2" ht="44.1" customHeight="1">
       <c r="A210" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B210" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="44.1" customHeight="1">
       <c r="A211" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B211" s="7" t="s">
         <v>399</v>
-      </c>
-      <c r="B211" s="7" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="44.1" customHeight="1">
@@ -4029,10 +4044,10 @@
     </row>
     <row r="213" spans="1:2" ht="44.1" customHeight="1">
       <c r="A213" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B213" s="7" t="s">
         <v>401</v>
-      </c>
-      <c r="B213" s="7" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="44.1" customHeight="1">
@@ -4040,79 +4055,79 @@
         <v>333</v>
       </c>
       <c r="B214" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="44.1" customHeight="1">
       <c r="A215" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="B215" s="7" t="s">
         <v>404</v>
-      </c>
-      <c r="B215" s="7" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="44.1" customHeight="1">
       <c r="A216" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="B216" s="7" t="s">
         <v>406</v>
-      </c>
-      <c r="B216" s="7" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="44.1" customHeight="1">
       <c r="A217" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B217" s="7" t="s">
         <v>408</v>
-      </c>
-      <c r="B217" s="7" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="44.1" customHeight="1">
       <c r="A218" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B218" s="7" t="s">
         <v>410</v>
-      </c>
-      <c r="B218" s="7" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="44.1" customHeight="1">
       <c r="A219" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B219" s="7" t="s">
         <v>412</v>
-      </c>
-      <c r="B219" s="7" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="44.1" customHeight="1">
       <c r="A220" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B220" s="7" t="s">
         <v>414</v>
-      </c>
-      <c r="B220" s="7" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="44.1" customHeight="1">
       <c r="A221" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B221" s="7" t="s">
         <v>416</v>
-      </c>
-      <c r="B221" s="7" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="44.1" customHeight="1">
       <c r="A222" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B222" s="7" t="s">
         <v>418</v>
-      </c>
-      <c r="B222" s="7" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="44.1" customHeight="1">
       <c r="A223" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B223" s="7" t="s">
         <v>420</v>
-      </c>
-      <c r="B223" s="7" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="44.1" customHeight="1">
@@ -4125,23 +4140,23 @@
     </row>
     <row r="225" spans="1:2" ht="44.1" customHeight="1">
       <c r="A225" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="B225" s="7" t="s">
         <v>422</v>
-      </c>
-      <c r="B225" s="7" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="44.1" customHeight="1">
       <c r="A226" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B226" s="7" t="s">
         <v>424</v>
-      </c>
-      <c r="B226" s="7" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="44.1" customHeight="1">
       <c r="A227" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B227" s="7" t="s">
         <v>315</v>
@@ -4149,66 +4164,66 @@
     </row>
     <row r="228" spans="1:2" ht="44.1" customHeight="1">
       <c r="A228" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="44.1" customHeight="1">
       <c r="A229" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B229" s="7" t="s">
         <v>428</v>
-      </c>
-      <c r="B229" s="7" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="44.1" customHeight="1">
       <c r="A230" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="B230" s="7" t="s">
         <v>430</v>
-      </c>
-      <c r="B230" s="7" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="44.1" customHeight="1">
       <c r="A231" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="B231" s="7" t="s">
         <v>432</v>
-      </c>
-      <c r="B231" s="7" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="44.1" customHeight="1">
       <c r="A232" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B232" s="7" t="s">
         <v>434</v>
-      </c>
-      <c r="B232" s="7" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="44.1" customHeight="1">
       <c r="A233" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="B233" s="7" t="s">
         <v>436</v>
-      </c>
-      <c r="B233" s="7" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="44.1" customHeight="1">
       <c r="A234" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B234" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="44.1" customHeight="1">
       <c r="A235" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B235" s="7" t="s">
         <v>439</v>
-      </c>
-      <c r="B235" s="7" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="44.1" customHeight="1">
@@ -4216,23 +4231,23 @@
         <v>333</v>
       </c>
       <c r="B236" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="44.1" customHeight="1">
       <c r="A237" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B237" s="7" t="s">
         <v>442</v>
-      </c>
-      <c r="B237" s="7" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="44.1" customHeight="1">
       <c r="A238" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="B238" s="7" t="s">
         <v>444</v>
-      </c>
-      <c r="B238" s="7" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="44.1" customHeight="1">
@@ -4240,191 +4255,191 @@
         <v>335</v>
       </c>
       <c r="B239" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="44.1" customHeight="1">
       <c r="A240" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B240" s="7" t="s">
         <v>447</v>
-      </c>
-      <c r="B240" s="7" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="44.1" customHeight="1">
       <c r="A241" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="B241" s="7" t="s">
         <v>449</v>
-      </c>
-      <c r="B241" s="7" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="44.1" customHeight="1">
       <c r="A242" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="B242" s="7" t="s">
         <v>451</v>
-      </c>
-      <c r="B242" s="7" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="44.1" customHeight="1">
       <c r="A243" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="B243" s="7" t="s">
         <v>453</v>
-      </c>
-      <c r="B243" s="7" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="44.1" customHeight="1">
       <c r="A244" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="B244" s="7" t="s">
         <v>455</v>
-      </c>
-      <c r="B244" s="7" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="44.1" customHeight="1">
       <c r="A245" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="B245" s="7" t="s">
         <v>457</v>
-      </c>
-      <c r="B245" s="7" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="44.1" customHeight="1">
       <c r="A246" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="B246" s="7" t="s">
         <v>459</v>
-      </c>
-      <c r="B246" s="7" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="44.1" customHeight="1">
       <c r="A247" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="B247" s="7" t="s">
         <v>461</v>
-      </c>
-      <c r="B247" s="7" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="44.1" customHeight="1">
       <c r="A248" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="B248" s="7" t="s">
         <v>463</v>
-      </c>
-      <c r="B248" s="7" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="44.1" customHeight="1">
       <c r="A249" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="B249" s="7" t="s">
         <v>465</v>
-      </c>
-      <c r="B249" s="7" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="44.1" customHeight="1">
       <c r="A250" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B250" s="7" t="s">
         <v>467</v>
-      </c>
-      <c r="B250" s="7" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="44.1" customHeight="1">
       <c r="A251" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="B251" s="7" t="s">
         <v>406</v>
-      </c>
-      <c r="B251" s="7" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="44.1" customHeight="1">
       <c r="A252" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="B252" s="7" t="s">
         <v>469</v>
-      </c>
-      <c r="B252" s="7" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="44.1" customHeight="1">
       <c r="A253" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="B253" s="7" t="s">
         <v>471</v>
-      </c>
-      <c r="B253" s="7" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="44.1" customHeight="1">
       <c r="A254" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="B254" s="7" t="s">
         <v>473</v>
-      </c>
-      <c r="B254" s="7" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="44.1" customHeight="1">
       <c r="A255" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B255" s="18" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="87" customHeight="1">
       <c r="A256" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="B256" s="17" t="s">
         <v>476</v>
-      </c>
-      <c r="B256" s="17" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="44.1" customHeight="1">
       <c r="A257" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="B257" s="7" t="s">
         <v>479</v>
-      </c>
-      <c r="B257" s="7" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="44.1" customHeight="1">
       <c r="A258" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="B258" s="7" t="s">
         <v>481</v>
-      </c>
-      <c r="B258" s="7" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="44.1" customHeight="1">
       <c r="A259" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="B259" s="7" t="s">
         <v>483</v>
-      </c>
-      <c r="B259" s="7" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="44.1" customHeight="1">
       <c r="A260" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="B260" s="7" t="s">
         <v>485</v>
-      </c>
-      <c r="B260" s="7" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="44.1" customHeight="1">
       <c r="A261" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B261" s="7" t="s">
         <v>487</v>
-      </c>
-      <c r="B261" s="7" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="44.1" customHeight="1">
       <c r="A262" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="B262" s="7" t="s">
         <v>489</v>
-      </c>
-      <c r="B262" s="7" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="44.1" customHeight="1">
@@ -4437,175 +4452,187 @@
     </row>
     <row r="264" spans="1:2" ht="44.1" customHeight="1">
       <c r="A264" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="B264" s="7" t="s">
         <v>491</v>
-      </c>
-      <c r="B264" s="7" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="44.1" customHeight="1">
       <c r="A265" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B265" s="7" t="s">
         <v>493</v>
-      </c>
-      <c r="B265" s="7" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="44.1" customHeight="1">
       <c r="A266" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B266" s="7" t="s">
         <v>495</v>
-      </c>
-      <c r="B266" s="7" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="44.1" customHeight="1">
       <c r="A267" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B267" s="7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="44.1" customHeight="1">
       <c r="A268" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="B268" s="7" t="s">
         <v>498</v>
-      </c>
-      <c r="B268" s="7" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="44.1" customHeight="1">
       <c r="A269" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B269" s="7" t="s">
         <v>500</v>
-      </c>
-      <c r="B269" s="7" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="44.1" customHeight="1">
       <c r="A270" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="B270" s="7" t="s">
         <v>502</v>
-      </c>
-      <c r="B270" s="7" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="44.1" customHeight="1">
       <c r="A271" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B271" s="7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="44.1" customHeight="1">
       <c r="A272" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="B272" s="7" t="s">
         <v>506</v>
-      </c>
-      <c r="B272" s="7" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="44.1" customHeight="1">
       <c r="A273" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="B273" s="7" t="s">
         <v>508</v>
-      </c>
-      <c r="B273" s="7" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="44.1" customHeight="1">
       <c r="A274" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="B274" s="7" t="s">
         <v>510</v>
-      </c>
-      <c r="B274" s="7" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="44.1" customHeight="1">
       <c r="A275" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="B275" s="7" t="s">
         <v>512</v>
-      </c>
-      <c r="B275" s="7" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="44.1" customHeight="1">
       <c r="A276" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="B276" s="7" t="s">
         <v>514</v>
-      </c>
-      <c r="B276" s="7" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="44.1" customHeight="1">
       <c r="A277" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="B277" s="7" t="s">
         <v>516</v>
-      </c>
-      <c r="B277" s="7" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="44.1" customHeight="1">
       <c r="A278" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="B278" s="7" t="s">
         <v>518</v>
-      </c>
-      <c r="B278" s="7" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="44.1" customHeight="1">
       <c r="A279" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="B279" s="7" t="s">
         <v>520</v>
-      </c>
-      <c r="B279" s="7" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="44.1" customHeight="1">
       <c r="A280" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="B280" s="7" t="s">
         <v>522</v>
-      </c>
-      <c r="B280" s="7" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="44.1" customHeight="1">
       <c r="A281" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="B281" s="7" t="s">
         <v>524</v>
-      </c>
-      <c r="B281" s="7" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="44.1" customHeight="1">
       <c r="A282" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="B282" s="7" t="s">
         <v>526</v>
-      </c>
-      <c r="B282" s="7" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="44.1" customHeight="1">
       <c r="A283" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="B283" s="7" t="s">
         <v>528</v>
       </c>
-      <c r="B283" s="7" t="s">
+    </row>
+    <row r="284" spans="1:2" ht="44.1" customHeight="1">
+      <c r="A284" s="3" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="284" spans="1:2" ht="44.1" customHeight="1">
-      <c r="A284" s="3"/>
-      <c r="B284" s="7"/>
+      <c r="B284" s="7" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="285" spans="1:2" ht="44.1" customHeight="1">
-      <c r="A285" s="3"/>
-      <c r="B285" s="7"/>
+      <c r="A285" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="B285" s="7" t="s">
+        <v>532</v>
+      </c>
     </row>
     <row r="286" spans="1:2" ht="44.1" customHeight="1">
-      <c r="A286" s="3"/>
-      <c r="B286" s="7"/>
+      <c r="A286" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="B286" s="7" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="287" spans="1:2" ht="44.1" customHeight="1">
       <c r="A287" s="3"/>

</xml_diff>